<commit_message>
undid my Georgia "fix" and reran, plus 4b-5a reorder
</commit_message>
<xml_diff>
--- a/output/table2.xlsx
+++ b/output/table2.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="102" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="136" uniqueCount="11">
   <si>
     <t>Panel 1: All Gymnasts</t>
   </si>
@@ -55,7 +55,727 @@
   <numFmts count="1">
     <numFmt numFmtId="166" formatCode="#0.00"/>
   </numFmts>
-  <fonts count="541">
+  <fonts count="721">
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -2229,7 +2949,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="541">
+  <borders count="721">
     <border>
       <left/>
       <right/>
@@ -6017,11 +6737,1271 @@
       <bottom style="none"/>
       <diagonal style="none"/>
     </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="541">
+  <cellXfs count="721">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
@@ -8180,6 +10160,726 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="540" fillId="0" borderId="540" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="541" fillId="0" borderId="541" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="542" fillId="0" borderId="542" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="543" fillId="0" borderId="543" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="544" fillId="0" borderId="544" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="545" fillId="0" borderId="545" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="546" fillId="0" borderId="546" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="547" fillId="0" borderId="547" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="548" fillId="0" borderId="548" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="549" fillId="0" borderId="549" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="550" fillId="0" borderId="550" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="551" fillId="0" borderId="551" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="552" fillId="0" borderId="552" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="553" fillId="0" borderId="553" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="554" fillId="0" borderId="554" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="555" fillId="0" borderId="555" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="556" fillId="0" borderId="556" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="557" fillId="0" borderId="557" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="558" fillId="0" borderId="558" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="559" fillId="0" borderId="559" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="560" fillId="0" borderId="560" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="561" fillId="0" borderId="561" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="562" fillId="0" borderId="562" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="563" fillId="0" borderId="563" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="564" fillId="0" borderId="564" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="565" fillId="0" borderId="565" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="566" fillId="0" borderId="566" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="567" fillId="0" borderId="567" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="568" fillId="0" borderId="568" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="569" fillId="0" borderId="569" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="570" fillId="0" borderId="570" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="571" fillId="0" borderId="571" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="572" fillId="0" borderId="572" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="573" fillId="0" borderId="573" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="574" fillId="0" borderId="574" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="575" fillId="0" borderId="575" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="576" fillId="0" borderId="576" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="577" fillId="0" borderId="577" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="578" fillId="0" borderId="578" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="579" fillId="0" borderId="579" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="580" fillId="0" borderId="580" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="581" fillId="0" borderId="581" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="582" fillId="0" borderId="582" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="583" fillId="0" borderId="583" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="584" fillId="0" borderId="584" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="585" fillId="0" borderId="585" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="586" fillId="0" borderId="586" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="587" fillId="0" borderId="587" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="588" fillId="0" borderId="588" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="589" fillId="0" borderId="589" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="590" fillId="0" borderId="590" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="591" fillId="0" borderId="591" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="592" fillId="0" borderId="592" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="593" fillId="0" borderId="593" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="594" fillId="0" borderId="594" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="595" fillId="0" borderId="595" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="596" fillId="0" borderId="596" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="597" fillId="0" borderId="597" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="598" fillId="0" borderId="598" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="599" fillId="0" borderId="599" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="600" fillId="0" borderId="600" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="601" fillId="0" borderId="601" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="602" fillId="0" borderId="602" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="603" fillId="0" borderId="603" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="604" fillId="0" borderId="604" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="605" fillId="0" borderId="605" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="606" fillId="0" borderId="606" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="607" fillId="0" borderId="607" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="608" fillId="0" borderId="608" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="609" fillId="0" borderId="609" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="610" fillId="0" borderId="610" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="611" fillId="0" borderId="611" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="612" fillId="0" borderId="612" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="613" fillId="0" borderId="613" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="614" fillId="0" borderId="614" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="615" fillId="0" borderId="615" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="616" fillId="0" borderId="616" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="617" fillId="0" borderId="617" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="618" fillId="0" borderId="618" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="619" fillId="0" borderId="619" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="620" fillId="0" borderId="620" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="621" fillId="0" borderId="621" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="622" fillId="0" borderId="622" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="623" fillId="0" borderId="623" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="624" fillId="0" borderId="624" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="625" fillId="0" borderId="625" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="626" fillId="0" borderId="626" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="627" fillId="0" borderId="627" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="628" fillId="0" borderId="628" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="629" fillId="0" borderId="629" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="630" fillId="0" borderId="630" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="631" fillId="0" borderId="631" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="632" fillId="0" borderId="632" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="633" fillId="0" borderId="633" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="634" fillId="0" borderId="634" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="635" fillId="0" borderId="635" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="636" fillId="0" borderId="636" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="637" fillId="0" borderId="637" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="638" fillId="0" borderId="638" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="639" fillId="0" borderId="639" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="640" fillId="0" borderId="640" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="641" fillId="0" borderId="641" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="642" fillId="0" borderId="642" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="643" fillId="0" borderId="643" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="644" fillId="0" borderId="644" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="645" fillId="0" borderId="645" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="646" fillId="0" borderId="646" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="647" fillId="0" borderId="647" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="648" fillId="0" borderId="648" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="649" fillId="0" borderId="649" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="650" fillId="0" borderId="650" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="651" fillId="0" borderId="651" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="652" fillId="0" borderId="652" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="653" fillId="0" borderId="653" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="654" fillId="0" borderId="654" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="655" fillId="0" borderId="655" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="656" fillId="0" borderId="656" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="657" fillId="0" borderId="657" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="658" fillId="0" borderId="658" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="659" fillId="0" borderId="659" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="660" fillId="0" borderId="660" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="661" fillId="0" borderId="661" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="662" fillId="0" borderId="662" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="663" fillId="0" borderId="663" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="664" fillId="0" borderId="664" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="665" fillId="0" borderId="665" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="666" fillId="0" borderId="666" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="667" fillId="0" borderId="667" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="668" fillId="0" borderId="668" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="669" fillId="0" borderId="669" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="670" fillId="0" borderId="670" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="671" fillId="0" borderId="671" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="672" fillId="0" borderId="672" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="673" fillId="0" borderId="673" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="674" fillId="0" borderId="674" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="675" fillId="0" borderId="675" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="676" fillId="0" borderId="676" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="677" fillId="0" borderId="677" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="678" fillId="0" borderId="678" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="679" fillId="0" borderId="679" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="680" fillId="0" borderId="680" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="681" fillId="0" borderId="681" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="682" fillId="0" borderId="682" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="683" fillId="0" borderId="683" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="684" fillId="0" borderId="684" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="685" fillId="0" borderId="685" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="686" fillId="0" borderId="686" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="687" fillId="0" borderId="687" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="688" fillId="0" borderId="688" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="689" fillId="0" borderId="689" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="690" fillId="0" borderId="690" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="691" fillId="0" borderId="691" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="692" fillId="0" borderId="692" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="693" fillId="0" borderId="693" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="694" fillId="0" borderId="694" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="695" fillId="0" borderId="695" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="696" fillId="0" borderId="696" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="697" fillId="0" borderId="697" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="698" fillId="0" borderId="698" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="699" fillId="0" borderId="699" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="700" fillId="0" borderId="700" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="701" fillId="0" borderId="701" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="702" fillId="0" borderId="702" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="703" fillId="0" borderId="703" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="704" fillId="0" borderId="704" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="705" fillId="0" borderId="705" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="706" fillId="0" borderId="706" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="707" fillId="0" borderId="707" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="708" fillId="0" borderId="708" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="709" fillId="0" borderId="709" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="710" fillId="0" borderId="710" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="711" fillId="0" borderId="711" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="712" fillId="0" borderId="712" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="713" fillId="0" borderId="713" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="714" fillId="0" borderId="714" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="715" fillId="0" borderId="715" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="716" fillId="0" borderId="716" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="717" fillId="0" borderId="717" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="718" fillId="0" borderId="718" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="719" fillId="0" borderId="719" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="720" fillId="0" borderId="720" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -8224,36 +10924,36 @@
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="451">
+      <c r="B3" s="631">
         <v>9.6262788172613547</v>
       </c>
-      <c r="C3" s="452">
+      <c r="C3" s="632">
         <v>9.4985233712130785</v>
       </c>
-      <c r="D3" s="453">
+      <c r="D3" s="633">
         <v>9.5310703563207682</v>
       </c>
-      <c r="E3" s="454">
+      <c r="E3" s="634">
         <v>9.6185530142109492</v>
       </c>
-      <c r="F3" s="455">
+      <c r="F3" s="635">
         <v>9.5677677699685333</v>
       </c>
     </row>
     <row r="4">
-      <c r="B4" s="456">
+      <c r="B4" s="636">
         <v>0.26629049823736922</v>
       </c>
-      <c r="C4" s="457">
+      <c r="C4" s="637">
         <v>0.50950401995643524</v>
       </c>
-      <c r="D4" s="458">
+      <c r="D4" s="638">
         <v>0.41699738504902423</v>
       </c>
-      <c r="E4" s="459">
+      <c r="E4" s="639">
         <v>0.37779434640592702</v>
       </c>
-      <c r="F4" s="460">
+      <c r="F4" s="640">
         <v>0.40737844003334822</v>
       </c>
     </row>
@@ -8261,36 +10961,36 @@
       <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="461">
+      <c r="B5" s="641">
         <v>9.6995065786728727</v>
       </c>
-      <c r="C5" s="462">
+      <c r="C5" s="642">
         <v>9.6121464512722721</v>
       </c>
-      <c r="D5" s="463">
+      <c r="D5" s="643">
         <v>9.595921749324031</v>
       </c>
-      <c r="E5" s="464">
+      <c r="E5" s="644">
         <v>9.709897872639381</v>
       </c>
-      <c r="F5" s="465">
+      <c r="F5" s="645">
         <v>9.6622813323634009</v>
       </c>
     </row>
     <row r="6">
-      <c r="B6" s="466">
+      <c r="B6" s="646">
         <v>0.23880230199483959</v>
       </c>
-      <c r="C6" s="467">
+      <c r="C6" s="647">
         <v>0.45160002240660252</v>
       </c>
-      <c r="D6" s="468">
+      <c r="D6" s="648">
         <v>0.36758700082789431</v>
       </c>
-      <c r="E6" s="469">
+      <c r="E6" s="649">
         <v>0.33722675120036089</v>
       </c>
-      <c r="F6" s="470">
+      <c r="F6" s="650">
         <v>0.35116915193077392</v>
       </c>
     </row>
@@ -8298,36 +10998,36 @@
       <c r="A7" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="471">
+      <c r="B7" s="651">
         <v>9.6444806606527678</v>
       </c>
-      <c r="C7" s="472">
+      <c r="C7" s="652">
         <v>9.5260273873515207</v>
       </c>
-      <c r="D7" s="473">
+      <c r="D7" s="653">
         <v>9.5564048631271312</v>
       </c>
-      <c r="E7" s="474">
+      <c r="E7" s="654">
         <v>9.6381783656526707</v>
       </c>
-      <c r="F7" s="475">
+      <c r="F7" s="655">
         <v>9.5911624582714943</v>
       </c>
     </row>
     <row r="8">
-      <c r="B8" s="476">
+      <c r="B8" s="656">
         <v>0.25858677687265907</v>
       </c>
-      <c r="C8" s="477">
+      <c r="C8" s="657">
         <v>0.49589567389843331</v>
       </c>
-      <c r="D8" s="478">
+      <c r="D8" s="658">
         <v>0.40160827568108193</v>
       </c>
-      <c r="E8" s="479">
+      <c r="E8" s="659">
         <v>0.37285527634968341</v>
       </c>
-      <c r="F8" s="480">
+      <c r="F8" s="660">
         <v>0.39496689732178619</v>
       </c>
     </row>
@@ -8340,36 +11040,36 @@
       <c r="A11" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="481">
+      <c r="B11" s="661">
         <v>9.7158729720477091</v>
       </c>
-      <c r="C11" s="482">
+      <c r="C11" s="662">
         <v>9.6522917370928454</v>
       </c>
-      <c r="D11" s="483">
+      <c r="D11" s="663">
         <v>9.6504889986637696</v>
       </c>
-      <c r="E11" s="484">
+      <c r="E11" s="664">
         <v>9.7102592437321906</v>
       </c>
-      <c r="F11" s="485">
+      <c r="F11" s="665">
         <v>9.6817795138661076</v>
       </c>
     </row>
     <row r="12">
-      <c r="B12" s="486">
+      <c r="B12" s="666">
         <v>0.1835039086205251</v>
       </c>
-      <c r="C12" s="487">
+      <c r="C12" s="667">
         <v>0.36638046840985983</v>
       </c>
-      <c r="D12" s="488">
+      <c r="D12" s="668">
         <v>0.30744455013892441</v>
       </c>
-      <c r="E12" s="489">
+      <c r="E12" s="669">
         <v>0.3144581307202618</v>
       </c>
-      <c r="F12" s="490">
+      <c r="F12" s="670">
         <v>0.30321582241459177</v>
       </c>
     </row>
@@ -8377,36 +11077,36 @@
       <c r="A13" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="491">
+      <c r="B13" s="671">
         <v>9.7536332184173542</v>
       </c>
-      <c r="C13" s="492">
+      <c r="C13" s="672">
         <v>9.6980953895717956</v>
       </c>
-      <c r="D13" s="493">
+      <c r="D13" s="673">
         <v>9.6708576311076584</v>
       </c>
-      <c r="E13" s="494">
+      <c r="E13" s="674">
         <v>9.7611590072504466</v>
       </c>
-      <c r="F13" s="495">
+      <c r="F13" s="675">
         <v>9.7270729845677035</v>
       </c>
     </row>
     <row r="14">
-      <c r="B14" s="496">
+      <c r="B14" s="676">
         <v>0.18350999306875629</v>
       </c>
-      <c r="C14" s="497">
+      <c r="C14" s="677">
         <v>0.36827594017943499</v>
       </c>
-      <c r="D14" s="498">
+      <c r="D14" s="678">
         <v>0.29395556844565418</v>
       </c>
-      <c r="E14" s="499">
+      <c r="E14" s="679">
         <v>0.27927946408178511</v>
       </c>
-      <c r="F14" s="500">
+      <c r="F14" s="680">
         <v>0.28379594196863589</v>
       </c>
     </row>
@@ -8414,36 +11114,36 @@
       <c r="A15" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="501">
+      <c r="B15" s="681">
         <v>9.723498025870823</v>
       </c>
-      <c r="C15" s="502">
+      <c r="C15" s="682">
         <v>9.6612851288534678</v>
       </c>
-      <c r="D15" s="503">
+      <c r="D15" s="683">
         <v>9.6598321843571711</v>
       </c>
-      <c r="E15" s="504">
+      <c r="E15" s="684">
         <v>9.7199659287550624</v>
       </c>
-      <c r="F15" s="505">
+      <c r="F15" s="685">
         <v>9.6910642596827188</v>
       </c>
     </row>
     <row r="16">
-      <c r="B16" s="506">
+      <c r="B16" s="686">
         <v>0.18292438521802901</v>
       </c>
-      <c r="C16" s="507">
+      <c r="C16" s="687">
         <v>0.36787649978208831</v>
       </c>
-      <c r="D16" s="508">
+      <c r="D16" s="688">
         <v>0.30031803790445227</v>
       </c>
-      <c r="E16" s="509">
+      <c r="E16" s="689">
         <v>0.31184518996317839</v>
       </c>
-      <c r="F16" s="510">
+      <c r="F16" s="690">
         <v>0.30010201662005881</v>
       </c>
     </row>
@@ -8456,36 +11156,36 @@
       <c r="A19" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="511">
+      <c r="B19" s="691">
         <v>9.3761056774185612</v>
       </c>
-      <c r="C19" s="512">
+      <c r="C19" s="692">
         <v>9.0691393206063839</v>
       </c>
-      <c r="D19" s="513">
+      <c r="D19" s="693">
         <v>9.2002798917463267</v>
       </c>
-      <c r="E19" s="514">
+      <c r="E19" s="694">
         <v>9.3596483718988903</v>
       </c>
-      <c r="F19" s="515">
+      <c r="F19" s="695">
         <v>9.2491819905256865</v>
       </c>
     </row>
     <row r="20">
-      <c r="B20" s="516">
+      <c r="B20" s="696">
         <v>0.2998234963363996</v>
       </c>
-      <c r="C20" s="517">
+      <c r="C20" s="697">
         <v>0.59940468810912972</v>
       </c>
-      <c r="D20" s="518">
+      <c r="D20" s="698">
         <v>0.49479843076328178</v>
       </c>
-      <c r="E20" s="519">
+      <c r="E20" s="699">
         <v>0.41923087500805201</v>
       </c>
-      <c r="F20" s="520">
+      <c r="F20" s="700">
         <v>0.4847390578693534</v>
       </c>
     </row>
@@ -8493,36 +11193,36 @@
       <c r="A21" t="s">
         <v>2</v>
       </c>
-      <c r="B21" s="521">
+      <c r="B21" s="701">
         <v>9.4317848373450399</v>
       </c>
-      <c r="C21" s="522">
+      <c r="C21" s="702">
         <v>9.1420742687971703</v>
       </c>
-      <c r="D21" s="523">
+      <c r="D21" s="703">
         <v>9.2671501587682208</v>
       </c>
-      <c r="E21" s="524">
+      <c r="E21" s="704">
         <v>9.4434566409625162</v>
       </c>
-      <c r="F21" s="525">
+      <c r="F21" s="705">
         <v>9.3384449059643124</v>
       </c>
     </row>
     <row r="22">
-      <c r="B22" s="526">
+      <c r="B22" s="706">
         <v>0.29399819105127639</v>
       </c>
-      <c r="C22" s="527">
+      <c r="C22" s="707">
         <v>0.56271951795506725</v>
       </c>
-      <c r="D22" s="528">
+      <c r="D22" s="708">
         <v>0.46517644172356748</v>
       </c>
-      <c r="E22" s="529">
+      <c r="E22" s="709">
         <v>0.4636980552779878</v>
       </c>
-      <c r="F22" s="530">
+      <c r="F22" s="710">
         <v>0.45972707198778362</v>
       </c>
     </row>
@@ -8530,36 +11230,36 @@
       <c r="A23" t="s">
         <v>3</v>
       </c>
-      <c r="B23" s="531">
+      <c r="B23" s="711">
         <v>9.3816418056866642</v>
       </c>
-      <c r="C23" s="532">
+      <c r="C23" s="712">
         <v>9.0739350954442131</v>
       </c>
-      <c r="D23" s="533">
+      <c r="D23" s="713">
         <v>9.2122536474898382</v>
       </c>
-      <c r="E23" s="534">
+      <c r="E23" s="714">
         <v>9.3655745496664355</v>
       </c>
-      <c r="F23" s="535">
+      <c r="F23" s="715">
         <v>9.2582570849463224</v>
       </c>
     </row>
     <row r="24">
-      <c r="B24" s="536">
+      <c r="B24" s="716">
         <v>0.29688259815856449</v>
       </c>
-      <c r="C24" s="537">
+      <c r="C24" s="717">
         <v>0.59161566582926539</v>
       </c>
-      <c r="D24" s="538">
+      <c r="D24" s="718">
         <v>0.49381280403838768</v>
       </c>
-      <c r="E24" s="539">
+      <c r="E24" s="719">
         <v>0.42621921446863292</v>
       </c>
-      <c r="F24" s="540">
+      <c r="F24" s="720">
         <v>0.48129547266071732</v>
       </c>
     </row>

</xml_diff>